<commit_message>
fix : merge amount close-amount and add new malicious addr
</commit_message>
<xml_diff>
--- a/all_tx_VX6J-VKYY.xlsx
+++ b/all_tx_VX6J-VKYY.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="47">
   <si>
     <t>date UTC</t>
   </si>
@@ -858,8 +858,8 @@
       <c r="D20">
         <v>0</v>
       </c>
-      <c r="E20">
-        <v>0</v>
+      <c r="E20" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:5">

</xml_diff>